<commit_message>
File for Test -v:3
</commit_message>
<xml_diff>
--- a/exel_doc/Result1.xlsx
+++ b/exel_doc/Result1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,70 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>FDTK1CB7140</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Неверный</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>DPTWNT8K140</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ПройденоУспех</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>фыв</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Неверный</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>asf</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Неверный</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>